<commit_message>
Visualization of embedding space and clustering
</commit_message>
<xml_diff>
--- a/downstream/utils/cell_type_color.xlsx
+++ b/downstream/utils/cell_type_color.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>Cell Type</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>Transitional B cells; soft, related to B cells but distinct.</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>#808080</t>
+  </si>
+  <si>
+    <t>Gray</t>
   </si>
   <si>
     <t>PVL</t>
@@ -560,7 +569,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -834,8 +843,20 @@
       <c r="C19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+      <c r="A20" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>